<commit_message>
V1.0, with updated and cleaned code, and new comments
</commit_message>
<xml_diff>
--- a/ROC_Analysis/ROC_TestResults.xlsx
+++ b/ROC_Analysis/ROC_TestResults.xlsx
@@ -179,11 +179,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Class Probability</a:t>
+              <a:t>Logistic</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Boundary Averages</a:t>
+              <a:t> Regression Model Results vs. Class Probability Cutoff</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -228,11 +228,8 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>0.05</c:v>
-          </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="76200" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -245,7 +242,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="9525">
+              <a:ln w="38100">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
@@ -255,24 +252,129 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$54</c:f>
+              <c:f>(Sheet1!$B$54,Sheet1!$E$54,Sheet1!$H$54,Sheet1!$K$54,Sheet1!$N$54,Sheet1!$Q$54,Sheet1!$T$54,Sheet1!$W$54,Sheet1!$AC$54,Sheet1!$AF$54,Sheet1!$AI$54,Sheet1!$AL$54,Sheet1!$AO$54,Sheet1!$AR$54,Sheet1!$AU$54,Sheet1!$AX$54,Sheet1!$BA$54,Sheet1!$BD$54)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0.23749999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.155</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1525</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.115</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.7500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.2499999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$54</c:f>
+              <c:f>(Sheet1!$A$54,Sheet1!$D$54,Sheet1!$G$54,Sheet1!$J$54,Sheet1!$M$54,Sheet1!$P$54,Sheet1!$S$54,Sheet1!$V$54,Sheet1!$Y$54,Sheet1!$AB$54,Sheet1!$AE$54,Sheet1!$AH$54,Sheet1!$AK$54,Sheet1!$AN$54,Sheet1!$AQ$54,Sheet1!$AT$54,Sheet1!$AW$54,Sheet1!$AZ$54,Sheet1!$BC$54)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>0.748</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80199999999999971</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80599999999999983</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82399999999999973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80799999999999972</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.78799999999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.79399999999999982</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78399999999999981</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.746</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.75399999999999978</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.79400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.7799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.75799999999999979</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7759999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.79599999999999993</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.73199999999999987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.73199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.73200000000000021</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,1133 +382,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>0.1</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.80199999999999971</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>0.15</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.155</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.80599999999999983</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000010-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>0.2</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$K$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.16250000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.82399999999999973</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000011-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>0.25</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$N$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.155</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$M$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.80799999999999972</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000012-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>0.3</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$Q$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.13</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$P$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.77800000000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000013-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>0.35</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$T$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.1525</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$S$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.78799999999999992</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000014-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:v>0.4</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$W$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.12</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$V$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.79399999999999982</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000015-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:v>0.45</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$Z$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.1275</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$Y$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.78399999999999981</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000016-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:v>0.5</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AC$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>7.4999999999999997E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AB$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.746</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000017-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
-          <c:tx>
-            <c:v>0.55</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AF$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.09</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AE$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.75399999999999978</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000018-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:v>0.6</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AI$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.115</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AH$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.79400000000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000019-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="12"/>
-          <c:order val="12"/>
-          <c:tx>
-            <c:v>0.65</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="80000"/>
-                    <a:lumOff val="20000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AL$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.105</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AK$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.7799999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001A-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="13"/>
-          <c:order val="13"/>
-          <c:tx>
-            <c:v>0.7</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="80000"/>
-                    <a:lumOff val="20000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AO$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.09</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AN$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.75799999999999979</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001B-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="14"/>
-          <c:order val="14"/>
-          <c:tx>
-            <c:v>0.75</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="80000"/>
-                    <a:lumOff val="20000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AR$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5.7500000000000002E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AQ$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.7759999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001C-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="15"/>
-          <c:order val="15"/>
-          <c:tx>
-            <c:v>0.8</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="80000"/>
-                    <a:lumOff val="20000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AU$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>7.2499999999999995E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AT$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.79599999999999993</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001D-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="16"/>
-          <c:order val="16"/>
-          <c:tx>
-            <c:v>0.85</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="80000"/>
-                    <a:lumOff val="20000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$AX$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5.5E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AW$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.73199999999999987</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001E-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="17"/>
-          <c:order val="17"/>
-          <c:tx>
-            <c:v>0.9</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="80000"/>
-                  <a:lumOff val="20000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="80000"/>
-                    <a:lumOff val="20000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$BA$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>6.5000000000000002E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$AZ$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.73199999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000001F-5BA0-4D3B-9561-3377125B649A}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="18"/>
-          <c:order val="18"/>
-          <c:tx>
-            <c:v>0.95</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="80000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="80000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$BD$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>6.25E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$BC$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0.73200000000000021</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000020-5BA0-4D3B-9561-3377125B649A}"/>
+              <c16:uniqueId val="{00000000-EC92-4D54-AC89-030E3480BF12}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1450,7 +426,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1463,7 +439,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>FPR</a:t>
                 </a:r>
               </a:p>
@@ -1483,7 +459,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1521,7 +497,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1583,7 +559,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" b="1"/>
                   <a:t>TPR</a:t>
                 </a:r>
               </a:p>
@@ -1641,7 +617,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -27411,8 +26387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AV54" sqref="AV54"/>
+    <sheetView tabSelected="1" topLeftCell="AU4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BE5" sqref="BE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>